<commit_message>
FB_010 add method for report(apache poi), kafka edited, add email message after booking to product module, add method for review after booking to rent module
</commit_message>
<xml_diff>
--- a/report_template.xlsx
+++ b/report_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\IdeaProjects\rent_apartment_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600DEB77-03A8-4737-999E-4F7A776A5F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF67F8F6-191B-4A0F-9D30-CB70519B2294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="18">
   <si>
     <t>Дата бронирования</t>
   </si>
@@ -55,6 +55,30 @@
   </si>
   <si>
     <t>Общая сумма выручки в отчетный месяц</t>
+  </si>
+  <si>
+    <t>2023-09-15 по 2023-09-21</t>
+  </si>
+  <si>
+    <t>slf4g</t>
+  </si>
+  <si>
+    <t>Москва Ленина 25</t>
+  </si>
+  <si>
+    <t>boxing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Омск Космический проспект 13</t>
+  </si>
+  <si>
+    <t>Омск Кордная 19</t>
+  </si>
+  <si>
+    <t>Новосибирск Хмельницкого 13</t>
   </si>
 </sst>
 </file>
@@ -372,19 +396,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="31.140625" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" customWidth="1"/>
@@ -424,6 +448,506 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>24225</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>28500</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>28500</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>28500</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>28500</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>15390</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>18240</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>18240</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>18240</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>18240</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>18240</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>18240</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>18240</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>22800</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>22800</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>22800</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>22800</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>22800</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>-72960</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20">
+        <v>500</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FB_012 add all controller methods from rent and product modules to application properties in proxy module
</commit_message>
<xml_diff>
--- a/report_template.xlsx
+++ b/report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\IdeaProjects\rent_apartment_app\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="22">
   <si>
     <t>Дата бронирования</t>
   </si>
@@ -79,12 +79,25 @@
   </si>
   <si>
     <t>Новосибирск Хмельницкого 13</t>
+  </si>
+  <si>
+    <t>testUser</t>
+  </si>
+  <si>
+    <t>Краснодар Столовая 3</t>
+  </si>
+  <si>
+    <t>Пенза Рабочая 17</t>
+  </si>
+  <si>
+    <t>Тверь Тверская 15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,16 +417,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="40.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="25.0"/>
+    <col min="2" max="2" customWidth="true" width="27.28515625"/>
+    <col min="3" max="3" customWidth="true" width="33.140625"/>
+    <col min="4" max="4" customWidth="true" width="11.85546875"/>
+    <col min="5" max="5" customWidth="true" width="40.7109375"/>
+    <col min="6" max="6" customWidth="true" width="21.140625"/>
+    <col min="7" max="7" customWidth="true" width="31.140625"/>
+    <col min="8" max="8" customWidth="true" width="20.28515625"/>
+    <col min="9" max="9" customWidth="true" width="20.42578125"/>
+    <col min="10" max="10" customWidth="true" width="40.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -448,135 +461,152 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>24225</v>
+      <c r="B2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15504.0</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="G2" t="n">
+        <v>15.0</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
       </c>
+      <c r="I2"/>
       <c r="J2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>28500</v>
+      <c r="B3" t="n">
+        <v>372.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1145016.0</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10.0</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
       </c>
+      <c r="I3"/>
       <c r="J3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>28500</v>
+      <c r="B4" t="n">
+        <v>372.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>699732.0</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12.0</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
       </c>
+      <c r="I4"/>
       <c r="J4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>28500</v>
+      <c r="B5" t="n">
+        <v>372.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>590884.8</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12.0</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
+      <c r="I5"/>
       <c r="J5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>28500</v>
+      <c r="B6" t="n">
+        <v>372.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1119571.2</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="G6" t="n">
+        <v>12.0</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
+      <c r="I6"/>
       <c r="J6" t="s">
         <v>14</v>
       </c>

</xml_diff>